<commit_message>
Adicionado tabelas para alimebtar banco em JSON
</commit_message>
<xml_diff>
--- a/banco_ditados.xlsx
+++ b/banco_ditados.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCASDOMINGOSLEAOGOM\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUCASDOMINGOSLEAOGOM\Desktop\Projetos\Tradutop-Novo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>id_giria</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>titulo</t>
   </si>
@@ -45,30 +42,32 @@
     <t>1</t>
   </si>
   <si>
-    <t>All mouth and no trousers</t>
-  </si>
-  <si>
-    <t>Toda a boca e sem calças.</t>
-  </si>
-  <si>
-    <t>Todas as conversas, sem ação.</t>
-  </si>
-  <si>
-    <t>Todas as Dont listen to him. Hes all mouth and no trousers, sem ação.</t>
-  </si>
-  <si>
-    <t>Não o escute. Ele é toda boca e sem calças.</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>Coloque os cavalos antes dos carros</t>
+  </si>
+  <si>
+    <t>Nao se precipitar</t>
+  </si>
+  <si>
+    <t>Put the horses before the cars</t>
+  </si>
+  <si>
+    <t>id_ditado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -96,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,13 +438,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet 1"/>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.125" bestFit="1" customWidth="1"/>
@@ -455,53 +455,55 @@
     <col min="7" max="7" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
       <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Banco de dados alimentados com registros
</commit_message>
<xml_diff>
--- a/banco_ditados.xlsx
+++ b/banco_ditados.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>titulo</t>
   </si>
@@ -42,16 +42,131 @@
     <t>1</t>
   </si>
   <si>
-    <t>Coloque os cavalos antes dos carros</t>
-  </si>
-  <si>
-    <t>Nao se precipitar</t>
-  </si>
-  <si>
-    <t>Put the horses before the cars</t>
-  </si>
-  <si>
     <t>id_ditado</t>
+  </si>
+  <si>
+    <t>Uma benção em disfarce</t>
+  </si>
+  <si>
+    <t>A blessing in disguise</t>
+  </si>
+  <si>
+    <t>Há males que vem para o bem</t>
+  </si>
+  <si>
+    <t>###</t>
+  </si>
+  <si>
+    <t>A chain is only as strong as its weakest link</t>
+  </si>
+  <si>
+    <t>Uma cadeia é tão forte quanto o link mais fraco</t>
+  </si>
+  <si>
+    <t>A corda sempre arrebenta no lado mais fraco</t>
+  </si>
+  <si>
+    <t>####</t>
+  </si>
+  <si>
+    <t>A close mouth catches no flies.</t>
+  </si>
+  <si>
+    <t>Uma boca próxima não pega moscas.</t>
+  </si>
+  <si>
+    <t>Boca fechada não entra mosca </t>
+  </si>
+  <si>
+    <t>A man is known by the company he keeps</t>
+  </si>
+  <si>
+    <t>Um homem é conhecido pela empresa que ele mantém</t>
+  </si>
+  <si>
+    <t>Diga com quem andas e te direi quem és</t>
+  </si>
+  <si>
+    <t>A word to the wise is enough.</t>
+  </si>
+  <si>
+    <t>Uma palavra para o sábio é suficiente.</t>
+  </si>
+  <si>
+    <t>Para bom entendedor meia palavra basta</t>
+  </si>
+  <si>
+    <t>All good things must come to an end.</t>
+  </si>
+  <si>
+    <t>Todas as coisas boas devem chegar ao fim.</t>
+  </si>
+  <si>
+    <t>Tudo o que é bom dura pouco</t>
+  </si>
+  <si>
+    <t>Barking dogs seldom bite.</t>
+  </si>
+  <si>
+    <t>Cão que ladra não morde.</t>
+  </si>
+  <si>
+    <r>
+      <t>Cachorro que late não morde</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF505050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Better alone than in bad company.</t>
+  </si>
+  <si>
+    <t>Melhor sozinho do que mal acompanhado.</t>
+  </si>
+  <si>
+    <t>Antes só do que mal acompanhado</t>
+  </si>
+  <si>
+    <t>Better late than never.</t>
+  </si>
+  <si>
+    <t>Antes tarde do que nunca.</t>
+  </si>
+  <si>
+    <t>Antes tarde do que nunca</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
@@ -67,12 +182,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF505050"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,9 +210,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,10 +552,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet 1"/>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -450,14 +564,14 @@
     <col min="2" max="2" width="22.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37" customWidth="1"/>
+    <col min="6" max="6" width="29.875" customWidth="1"/>
     <col min="7" max="7" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -478,7 +592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -486,21 +600,204 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G2">
         <v>3</v>
       </c>
-      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>